<commit_message>
Added Sample Tables as Excel
</commit_message>
<xml_diff>
--- a/Weapons - Inventory.xlsx
+++ b/Weapons - Inventory.xlsx
@@ -832,7 +832,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,35 +849,35 @@
     <col min="10" max="10" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>